<commit_message>
Updates to M2 and tables.
</commit_message>
<xml_diff>
--- a/_misc_docs/FormattedTables.xlsx
+++ b/_misc_docs/FormattedTables.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bacorli2/Documents/GitHub/scrna_workshop/_misc_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\GitHub\scrna_workshop\_misc_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FD30A5-38FE-2445-B10A-BA4E0AE161C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F455CC77-D6ED-483F-AB8C-F3346B6A9636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1840" windowWidth="29040" windowHeight="15720" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
   </bookViews>
   <sheets>
     <sheet name="CellType_Packages" sheetId="1" r:id="rId1"/>
     <sheet name="CellRanger_Output" sheetId="2" r:id="rId2"/>
+    <sheet name="Cell Ranger File Outputs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="88">
   <si>
     <t>Language</t>
   </si>
@@ -256,12 +257,90 @@
   <si>
     <t>CellTypeAnnotationReviewTable_Pasquini2021</t>
   </si>
+  <si>
+    <t>Run summary CSV</t>
+  </si>
+  <si>
+    <t>BAM</t>
+  </si>
+  <si>
+    <t>BAM index</t>
+  </si>
+  <si>
+    <t>Filtered feature-barcode matrices MEX</t>
+  </si>
+  <si>
+    <t>Filtered feature-barcode matrices HDF5</t>
+  </si>
+  <si>
+    <t>Unfiltered feature-barcode matrices MEX</t>
+  </si>
+  <si>
+    <t>Unfiltered feature-barcode matrices HDF5</t>
+  </si>
+  <si>
+    <t>Secondary analysis output CSV</t>
+  </si>
+  <si>
+    <t>Per-molecule read information</t>
+  </si>
+  <si>
+    <t>Loupe Browser file</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics_summary.csv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">possorted_genome_bam.bam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">possorted_genome_bam.bam.bai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">filtered_feature_bc_matrix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">filtered_feature_bc_matrix.h5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_feature_bc_matrix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_feature_bc_matrix_h5.h5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">analysis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">molecule_info.h5 </t>
+  </si>
+  <si>
+    <t>cloupe.cloupe</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Location: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./SRR23691690_ensemble/outs</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +375,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="SFMono-Regular"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF0A2347"/>
+      <name val="SFMono-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +411,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -447,27 +557,47 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF5F5F5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -778,27 +908,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A89453-62B7-439E-B590-76DBDC8D281E}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
-    <col min="9" max="9" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="42" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="36.75" customHeight="1" thickBot="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>53</v>
@@ -826,8 +956,8 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A3" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -849,8 +979,8 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A4" s="18"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -872,8 +1002,8 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A5" s="16"/>
       <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
@@ -895,8 +1025,8 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="11"/>
@@ -920,8 +1050,8 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A7" s="18"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
         <v>2</v>
@@ -943,8 +1073,8 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A8" s="18"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>2</v>
@@ -966,8 +1096,8 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A9" s="18"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
         <v>2</v>
@@ -989,8 +1119,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+    <row r="10" spans="1:10" ht="29.25" customHeight="1">
+      <c r="A10" s="18"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
         <v>2</v>
@@ -1010,8 +1140,8 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A11" s="16"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
         <v>2</v>
@@ -1031,8 +1161,8 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A12" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="11"/>
@@ -1054,8 +1184,8 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+    <row r="13" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A13" s="18"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -1075,8 +1205,8 @@
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A14" s="18"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
         <v>2</v>
@@ -1096,8 +1226,8 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+    <row r="15" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A15" s="18"/>
       <c r="B15" s="9" t="s">
         <v>2</v>
       </c>
@@ -1121,8 +1251,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+    <row r="16" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A16" s="18"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
@@ -1142,8 +1272,8 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
+    <row r="17" spans="1:9" ht="33.75" customHeight="1">
+      <c r="A17" s="16"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
         <v>2</v>
@@ -1167,8 +1297,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:9" ht="23.25" customHeight="1">
+      <c r="A18" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -1190,8 +1320,8 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
+    <row r="19" spans="1:9" ht="23.25" customHeight="1">
+      <c r="A19" s="16"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
         <v>2</v>
@@ -1211,7 +1341,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:9" ht="36.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A18:A19"/>
@@ -1227,101 +1357,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6003D3-9ACF-AC4E-B28D-DABB4461D7B6}">
   <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="4.83203125" customWidth="1"/>
+    <col min="1" max="5" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="13"/>
+      <c r="B3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1329,4 +1459,116 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB09241-04C8-4219-BC75-ED923D7ECE81}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="23" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="23" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A4" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1">
+      <c r="A5" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="23" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A6" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1">
+      <c r="A7" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="23" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A8" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17.25" customHeight="1">
+      <c r="A9" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="23" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A10" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.25" customHeight="1">
+      <c r="A11" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates M3, most of seurat pipeline slides are finished.
</commit_message>
<xml_diff>
--- a/_misc_docs/FormattedTables.xlsx
+++ b/_misc_docs/FormattedTables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\GitHub\scrna_workshop\_misc_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0E11CE-A6FF-40A3-9019-82123EC05E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB649F4-2F64-426E-A24D-31C4A996FCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
   </bookViews>
   <sheets>
     <sheet name="CellType_Packages" sheetId="1" r:id="rId1"/>
     <sheet name="CellRanger_Output" sheetId="2" r:id="rId2"/>
     <sheet name="Cell Ranger File Outputs" sheetId="3" r:id="rId3"/>
+    <sheet name="NearestNeighbors" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="97">
   <si>
     <t>Language</t>
   </si>
@@ -338,12 +339,36 @@
   <si>
     <t>…</t>
   </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Jackard</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Cell 1</t>
+  </si>
+  <si>
+    <t>Cell 2</t>
+  </si>
+  <si>
+    <t>Cell 3</t>
+  </si>
+  <si>
+    <t>Cell 4</t>
+  </si>
+  <si>
+    <t>E. Dist</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +428,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -424,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -648,11 +681,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -698,18 +746,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -722,12 +758,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,9 +826,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -792,7 +866,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -898,7 +972,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1040,7 +1114,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1099,7 +1173,7 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="33" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1122,7 +1196,7 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A4" s="22"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1145,7 +1219,7 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A5" s="20"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1168,7 +1242,7 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="11"/>
@@ -1193,7 +1267,7 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A7" s="22"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
         <v>2</v>
@@ -1216,7 +1290,7 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A8" s="22"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>2</v>
@@ -1239,7 +1313,7 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A9" s="22"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
         <v>2</v>
@@ -1262,7 +1336,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A10" s="22"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
         <v>2</v>
@@ -1283,7 +1357,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A11" s="20"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
         <v>2</v>
@@ -1304,7 +1378,7 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="31" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="11"/>
@@ -1327,7 +1401,7 @@
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A13" s="22"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -1348,7 +1422,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A14" s="22"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
         <v>2</v>
@@ -1369,7 +1443,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A15" s="22"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="9" t="s">
         <v>2</v>
       </c>
@@ -1394,7 +1468,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A16" s="22"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
@@ -1415,7 +1489,7 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A17" s="20"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
         <v>2</v>
@@ -1440,7 +1514,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="31" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -1463,7 +1537,7 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A19" s="20"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
         <v>2</v>
@@ -1499,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6003D3-9ACF-AC4E-B28D-DABB4461D7B6}">
   <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:D22"/>
     </sheetView>
   </sheetViews>
@@ -1515,54 +1589,54 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="12"/>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="29" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="27"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -1570,50 +1644,47 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="33"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
@@ -1621,47 +1692,47 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1774,4 +1845,473 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A855904-C17B-493C-A25B-56D1987B088F}">
+  <dimension ref="A2:S11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="2" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="13" width="6.42578125" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" customWidth="1"/>
+    <col min="15" max="15" width="2" customWidth="1"/>
+    <col min="16" max="16" width="4.7109375" customWidth="1"/>
+    <col min="17" max="18" width="6.42578125" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19">
+      <c r="A2" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q3" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="S3" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A4" s="39">
+        <v>1</v>
+      </c>
+      <c r="B4" s="35">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>324</v>
+      </c>
+      <c r="C4" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>0.95</v>
+      </c>
+      <c r="F4" s="39">
+        <v>1</v>
+      </c>
+      <c r="G4" s="35">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>531</v>
+      </c>
+      <c r="H4" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="I4">
+        <v>0.97</v>
+      </c>
+      <c r="K4" s="39">
+        <v>1</v>
+      </c>
+      <c r="L4" s="35">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>689</v>
+      </c>
+      <c r="M4" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="N4">
+        <v>0.99</v>
+      </c>
+      <c r="P4" s="39">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="35">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>358</v>
+      </c>
+      <c r="R4" s="35">
+        <v>0.12</v>
+      </c>
+      <c r="S4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A5" s="39">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35">
+        <f t="shared" ref="B5:B8" ca="1" si="0">RANDBETWEEN(1,1000)</f>
+        <v>90</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0.12</v>
+      </c>
+      <c r="D5">
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="39">
+        <v>2</v>
+      </c>
+      <c r="G5" s="35">
+        <f t="shared" ref="G5:G8" ca="1" si="1">RANDBETWEEN(1,1000)</f>
+        <v>535</v>
+      </c>
+      <c r="H5" s="35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.94</v>
+      </c>
+      <c r="K5" s="39">
+        <v>2</v>
+      </c>
+      <c r="L5" s="35">
+        <f t="shared" ref="L5:L8" ca="1" si="2">RANDBETWEEN(1,1000)</f>
+        <v>333</v>
+      </c>
+      <c r="M5" s="35">
+        <v>0.13</v>
+      </c>
+      <c r="N5">
+        <v>0.88</v>
+      </c>
+      <c r="P5" s="39">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="35">
+        <f t="shared" ref="Q5:Q8" ca="1" si="3">RANDBETWEEN(1,1000)</f>
+        <v>595</v>
+      </c>
+      <c r="R5" s="35">
+        <v>0.18</v>
+      </c>
+      <c r="S5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A6" s="39">
+        <v>3</v>
+      </c>
+      <c r="B6" s="35">
+        <f t="shared" ca="1" si="0"/>
+        <v>790</v>
+      </c>
+      <c r="C6" s="45">
+        <v>0.19</v>
+      </c>
+      <c r="D6">
+        <v>0.87</v>
+      </c>
+      <c r="F6" s="39">
+        <v>3</v>
+      </c>
+      <c r="G6" s="35">
+        <f t="shared" ca="1" si="1"/>
+        <v>845</v>
+      </c>
+      <c r="H6" s="35">
+        <v>0.11</v>
+      </c>
+      <c r="I6">
+        <v>0.89</v>
+      </c>
+      <c r="K6" s="39">
+        <v>3</v>
+      </c>
+      <c r="L6" s="35">
+        <f t="shared" ca="1" si="2"/>
+        <v>393</v>
+      </c>
+      <c r="M6" s="35">
+        <v>0.16</v>
+      </c>
+      <c r="N6">
+        <v>0.86</v>
+      </c>
+      <c r="P6" s="39">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="35">
+        <f t="shared" ca="1" si="3"/>
+        <v>861</v>
+      </c>
+      <c r="R6" s="35">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S6">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A7" s="39">
+        <v>4</v>
+      </c>
+      <c r="B7" s="35">
+        <f t="shared" ca="1" si="0"/>
+        <v>526</v>
+      </c>
+      <c r="C7" s="45">
+        <v>0.27</v>
+      </c>
+      <c r="D7">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="39">
+        <v>4</v>
+      </c>
+      <c r="G7" s="35">
+        <f t="shared" ca="1" si="1"/>
+        <v>932</v>
+      </c>
+      <c r="H7" s="35">
+        <v>0.21</v>
+      </c>
+      <c r="I7">
+        <v>0.83</v>
+      </c>
+      <c r="K7" s="39">
+        <v>4</v>
+      </c>
+      <c r="L7" s="35">
+        <f t="shared" ca="1" si="2"/>
+        <v>559</v>
+      </c>
+      <c r="M7" s="35">
+        <v>0.24</v>
+      </c>
+      <c r="N7">
+        <v>0.84</v>
+      </c>
+      <c r="P7" s="39">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="35">
+        <f t="shared" ca="1" si="3"/>
+        <v>847</v>
+      </c>
+      <c r="R7" s="35">
+        <v>0.31</v>
+      </c>
+      <c r="S7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A8" s="39">
+        <v>5</v>
+      </c>
+      <c r="B8" s="35">
+        <f t="shared" ca="1" si="0"/>
+        <v>153</v>
+      </c>
+      <c r="C8" s="45">
+        <v>0.34</v>
+      </c>
+      <c r="D8">
+        <v>0.82</v>
+      </c>
+      <c r="F8" s="39">
+        <v>5</v>
+      </c>
+      <c r="G8" s="35">
+        <f t="shared" ca="1" si="1"/>
+        <v>557</v>
+      </c>
+      <c r="H8" s="35">
+        <v>0.26</v>
+      </c>
+      <c r="I8">
+        <v>0.81</v>
+      </c>
+      <c r="K8" s="39">
+        <v>5</v>
+      </c>
+      <c r="L8" s="35">
+        <f t="shared" ca="1" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="M8" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="N8">
+        <v>0.82</v>
+      </c>
+      <c r="P8" s="39">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="35">
+        <f t="shared" ca="1" si="3"/>
+        <v>910</v>
+      </c>
+      <c r="R8" s="35">
+        <v>0.34</v>
+      </c>
+      <c r="S8">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A9" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="45"/>
+      <c r="F9" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="K9" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="P9" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+    </row>
+    <row r="10" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A10" s="39">
+        <v>20</v>
+      </c>
+      <c r="B10" s="35">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>162</v>
+      </c>
+      <c r="C10" s="45">
+        <v>1.3</v>
+      </c>
+      <c r="D10">
+        <v>0.7</v>
+      </c>
+      <c r="F10" s="43">
+        <v>20</v>
+      </c>
+      <c r="G10" s="29">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>730</v>
+      </c>
+      <c r="H10" s="29">
+        <v>1.2</v>
+      </c>
+      <c r="I10" s="42">
+        <v>0.74</v>
+      </c>
+      <c r="K10" s="43">
+        <v>20</v>
+      </c>
+      <c r="L10" s="29">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>54</v>
+      </c>
+      <c r="M10" s="29">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N10" s="42">
+        <v>0.6</v>
+      </c>
+      <c r="P10" s="43">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="29">
+        <f ca="1">RANDBETWEEN(1,1000)</f>
+        <v>420</v>
+      </c>
+      <c r="R10" s="29">
+        <v>3.4</v>
+      </c>
+      <c r="S10" s="42">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to M3 and formatted tables.
</commit_message>
<xml_diff>
--- a/_misc_docs/FormattedTables.xlsx
+++ b/_misc_docs/FormattedTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\GitHub\scrna_workshop\_misc_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB649F4-2F64-426E-A24D-31C4A996FCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF253E6B-AA91-4643-9093-4A7C481A5E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
   </bookViews>
@@ -1852,7 +1852,7 @@
   <dimension ref="A2:S11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="A2" sqref="A2:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B4" s="35">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>324</v>
+        <v>841</v>
       </c>
       <c r="C4" s="45">
         <v>0.04</v>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="G4" s="35">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>531</v>
+        <v>967</v>
       </c>
       <c r="H4" s="35">
         <v>0.02</v>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="L4" s="35">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>689</v>
+        <v>185</v>
       </c>
       <c r="M4" s="35">
         <v>0.8</v>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="Q4" s="35">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>358</v>
+        <v>61</v>
       </c>
       <c r="R4" s="35">
         <v>0.12</v>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B5" s="35">
         <f t="shared" ref="B5:B8" ca="1" si="0">RANDBETWEEN(1,1000)</f>
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C5" s="45">
         <v>0.12</v>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="G5" s="35">
         <f t="shared" ref="G5:G8" ca="1" si="1">RANDBETWEEN(1,1000)</f>
-        <v>535</v>
+        <v>426</v>
       </c>
       <c r="H5" s="35">
         <v>7.0000000000000007E-2</v>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="L5" s="35">
         <f t="shared" ref="L5:L8" ca="1" si="2">RANDBETWEEN(1,1000)</f>
-        <v>333</v>
+        <v>59</v>
       </c>
       <c r="M5" s="35">
         <v>0.13</v>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="Q5" s="35">
         <f t="shared" ref="Q5:Q8" ca="1" si="3">RANDBETWEEN(1,1000)</f>
-        <v>595</v>
+        <v>289</v>
       </c>
       <c r="R5" s="35">
         <v>0.18</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B6" s="35">
         <f t="shared" ca="1" si="0"/>
-        <v>790</v>
+        <v>651</v>
       </c>
       <c r="C6" s="45">
         <v>0.19</v>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="G6" s="35">
         <f t="shared" ca="1" si="1"/>
-        <v>845</v>
+        <v>393</v>
       </c>
       <c r="H6" s="35">
         <v>0.11</v>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="L6" s="35">
         <f t="shared" ca="1" si="2"/>
-        <v>393</v>
+        <v>60</v>
       </c>
       <c r="M6" s="35">
         <v>0.16</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="Q6" s="35">
         <f t="shared" ca="1" si="3"/>
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="R6" s="35">
         <v>0.28999999999999998</v>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B7" s="35">
         <f t="shared" ca="1" si="0"/>
-        <v>526</v>
+        <v>327</v>
       </c>
       <c r="C7" s="45">
         <v>0.27</v>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="G7" s="35">
         <f t="shared" ca="1" si="1"/>
-        <v>932</v>
+        <v>98</v>
       </c>
       <c r="H7" s="35">
         <v>0.21</v>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="L7" s="35">
         <f t="shared" ca="1" si="2"/>
-        <v>559</v>
+        <v>922</v>
       </c>
       <c r="M7" s="35">
         <v>0.24</v>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="Q7" s="35">
         <f t="shared" ca="1" si="3"/>
-        <v>847</v>
+        <v>374</v>
       </c>
       <c r="R7" s="35">
         <v>0.31</v>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="B8" s="35">
         <f t="shared" ca="1" si="0"/>
-        <v>153</v>
+        <v>273</v>
       </c>
       <c r="C8" s="45">
         <v>0.34</v>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="G8" s="35">
         <f t="shared" ca="1" si="1"/>
-        <v>557</v>
+        <v>673</v>
       </c>
       <c r="H8" s="35">
         <v>0.26</v>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="L8" s="35">
         <f t="shared" ca="1" si="2"/>
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="M8" s="35">
         <v>0.25</v>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="Q8" s="35">
         <f t="shared" ca="1" si="3"/>
-        <v>910</v>
+        <v>418</v>
       </c>
       <c r="R8" s="35">
         <v>0.34</v>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B10" s="35">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="C10" s="45">
         <v>1.3</v>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="G10" s="29">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>730</v>
+        <v>631</v>
       </c>
       <c r="H10" s="29">
         <v>1.2</v>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="L10" s="29">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>54</v>
+        <v>526</v>
       </c>
       <c r="M10" s="29">
         <v>2.2999999999999998</v>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="Q10" s="29">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>420</v>
+        <v>987</v>
       </c>
       <c r="R10" s="29">
         <v>3.4</v>

</xml_diff>

<commit_message>
Finishing M3 and reorganizing other modules.
</commit_message>
<xml_diff>
--- a/_misc_docs/FormattedTables.xlsx
+++ b/_misc_docs/FormattedTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\GitHub\scrna_workshop\_misc_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF253E6B-AA91-4643-9093-4A7C481A5E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737E235B-1431-4E47-A0F1-0BC8AC2B6459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{666724DD-9152-45AC-9376-DB960991B07F}"/>
   </bookViews>
   <sheets>
     <sheet name="CellType_Packages" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="97">
   <si>
     <t>Language</t>
   </si>
@@ -368,7 +368,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,8 +436,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,8 +464,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -563,129 +577,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -731,7 +622,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -746,35 +636,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -797,11 +660,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,7 +1076,7 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1196,7 +1099,7 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A4" s="34"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1219,7 +1122,7 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A5" s="32"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1145,7 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="11"/>
@@ -1267,7 +1170,7 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A7" s="34"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
         <v>2</v>
@@ -1290,7 +1193,7 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A8" s="34"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>2</v>
@@ -1313,7 +1216,7 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A9" s="34"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
         <v>2</v>
@@ -1336,7 +1239,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A10" s="34"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
         <v>2</v>
@@ -1357,7 +1260,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A11" s="32"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
         <v>2</v>
@@ -1378,7 +1281,7 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="11"/>
@@ -1401,7 +1304,7 @@
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A13" s="34"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
         <v>2</v>
@@ -1422,7 +1325,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A14" s="34"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
         <v>2</v>
@@ -1443,7 +1346,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A15" s="34"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="9" t="s">
         <v>2</v>
       </c>
@@ -1468,7 +1371,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A16" s="34"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
@@ -1489,7 +1392,7 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A17" s="32"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
         <v>2</v>
@@ -1514,7 +1417,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -1537,7 +1440,7 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A19" s="32"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
         <v>2</v>
@@ -1571,171 +1474,323 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6003D3-9ACF-AC4E-B28D-DABB4461D7B6}">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" s="45" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A2" s="44" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="12"/>
-      <c r="B3" s="29" t="s">
+    <row r="3" spans="1:6" ht="12" customHeight="1">
+      <c r="A3" s="36"/>
+      <c r="B3" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="33">
+        <v>0</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>15</v>
+      </c>
+      <c r="E4" s="35">
+        <v>3</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="33">
+        <v>5</v>
+      </c>
+      <c r="C5" s="33">
+        <v>2</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="35">
+        <v>0</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35">
+        <v>0</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="37" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="25" t="s">
+      <c r="B7" s="35">
+        <v>24</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="35">
+        <v>8</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="45" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A10" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="25" t="s">
+      <c r="B12" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="25" t="s">
+      <c r="B13" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="25" t="s">
+      <c r="B14" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="B15" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="45" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A18" s="44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="B18" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="25" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="36"/>
+      <c r="B19" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="34"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="25" t="s">
+      <c r="B20" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="25" t="s">
+      <c r="B21" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="25" t="s">
+      <c r="B22" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
+      <c r="B23" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1754,90 +1809,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A6" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A8" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A10" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1851,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A855904-C17B-493C-A25B-56D1987B088F}">
   <dimension ref="A2:S11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:S10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1875,132 +1930,132 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="44" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="44" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="44" t="s">
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="Q3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="40" t="s">
+      <c r="R3" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="S3" s="41" t="s">
+      <c r="S3" s="25" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A4" s="39">
+      <c r="A4" s="23">
         <v>1</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="19">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>841</v>
-      </c>
-      <c r="C4" s="45">
+        <v>107</v>
+      </c>
+      <c r="C4" s="19">
         <v>0.04</v>
       </c>
       <c r="D4">
         <v>0.95</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="19">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>967</v>
-      </c>
-      <c r="H4" s="35">
+        <v>909</v>
+      </c>
+      <c r="H4" s="19">
         <v>0.02</v>
       </c>
       <c r="I4">
         <v>0.97</v>
       </c>
-      <c r="K4" s="39">
+      <c r="K4" s="23">
         <v>1</v>
       </c>
-      <c r="L4" s="35">
+      <c r="L4" s="19">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>185</v>
-      </c>
-      <c r="M4" s="35">
+        <v>248</v>
+      </c>
+      <c r="M4" s="19">
         <v>0.8</v>
       </c>
       <c r="N4">
         <v>0.99</v>
       </c>
-      <c r="P4" s="39">
+      <c r="P4" s="23">
         <v>1</v>
       </c>
-      <c r="Q4" s="35">
+      <c r="Q4" s="19">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>61</v>
-      </c>
-      <c r="R4" s="35">
+        <v>843</v>
+      </c>
+      <c r="R4" s="19">
         <v>0.12</v>
       </c>
       <c r="S4">
@@ -2008,53 +2063,53 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A5" s="39">
+      <c r="A5" s="23">
         <v>2</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="19">
         <f t="shared" ref="B5:B8" ca="1" si="0">RANDBETWEEN(1,1000)</f>
-        <v>107</v>
-      </c>
-      <c r="C5" s="45">
+        <v>404</v>
+      </c>
+      <c r="C5" s="19">
         <v>0.12</v>
       </c>
       <c r="D5">
         <v>0.9</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="23">
         <v>2</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="19">
         <f t="shared" ref="G5:G8" ca="1" si="1">RANDBETWEEN(1,1000)</f>
-        <v>426</v>
-      </c>
-      <c r="H5" s="35">
+        <v>54</v>
+      </c>
+      <c r="H5" s="19">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I5">
         <v>0.94</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="23">
         <v>2</v>
       </c>
-      <c r="L5" s="35">
+      <c r="L5" s="19">
         <f t="shared" ref="L5:L8" ca="1" si="2">RANDBETWEEN(1,1000)</f>
-        <v>59</v>
-      </c>
-      <c r="M5" s="35">
+        <v>578</v>
+      </c>
+      <c r="M5" s="19">
         <v>0.13</v>
       </c>
       <c r="N5">
         <v>0.88</v>
       </c>
-      <c r="P5" s="39">
+      <c r="P5" s="23">
         <v>2</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="19">
         <f t="shared" ref="Q5:Q8" ca="1" si="3">RANDBETWEEN(1,1000)</f>
-        <v>289</v>
-      </c>
-      <c r="R5" s="35">
+        <v>738</v>
+      </c>
+      <c r="R5" s="19">
         <v>0.18</v>
       </c>
       <c r="S5">
@@ -2062,53 +2117,53 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A6" s="39">
+      <c r="A6" s="23">
         <v>3</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>651</v>
-      </c>
-      <c r="C6" s="45">
+        <v>575</v>
+      </c>
+      <c r="C6" s="19">
         <v>0.19</v>
       </c>
       <c r="D6">
         <v>0.87</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="23">
         <v>3</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>393</v>
-      </c>
-      <c r="H6" s="35">
+        <v>750</v>
+      </c>
+      <c r="H6" s="19">
         <v>0.11</v>
       </c>
       <c r="I6">
         <v>0.89</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="23">
         <v>3</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="M6" s="35">
+        <v>309</v>
+      </c>
+      <c r="M6" s="19">
         <v>0.16</v>
       </c>
       <c r="N6">
         <v>0.86</v>
       </c>
-      <c r="P6" s="39">
+      <c r="P6" s="23">
         <v>3</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>855</v>
-      </c>
-      <c r="R6" s="35">
+        <v>960</v>
+      </c>
+      <c r="R6" s="19">
         <v>0.28999999999999998</v>
       </c>
       <c r="S6">
@@ -2116,53 +2171,53 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A7" s="39">
+      <c r="A7" s="23">
         <v>4</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>327</v>
-      </c>
-      <c r="C7" s="45">
+        <v>412</v>
+      </c>
+      <c r="C7" s="19">
         <v>0.27</v>
       </c>
       <c r="D7">
         <v>0.85</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="23">
         <v>4</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="H7" s="35">
+        <v>142</v>
+      </c>
+      <c r="H7" s="19">
         <v>0.21</v>
       </c>
       <c r="I7">
         <v>0.83</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="23">
         <v>4</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>922</v>
-      </c>
-      <c r="M7" s="35">
+        <v>411</v>
+      </c>
+      <c r="M7" s="19">
         <v>0.24</v>
       </c>
       <c r="N7">
         <v>0.84</v>
       </c>
-      <c r="P7" s="39">
+      <c r="P7" s="23">
         <v>4</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>374</v>
-      </c>
-      <c r="R7" s="35">
+        <v>659</v>
+      </c>
+      <c r="R7" s="19">
         <v>0.31</v>
       </c>
       <c r="S7">
@@ -2170,53 +2225,53 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A8" s="39">
+      <c r="A8" s="23">
         <v>5</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>273</v>
-      </c>
-      <c r="C8" s="45">
+        <v>162</v>
+      </c>
+      <c r="C8" s="19">
         <v>0.34</v>
       </c>
       <c r="D8">
         <v>0.82</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="23">
         <v>5</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>673</v>
-      </c>
-      <c r="H8" s="35">
+        <v>57</v>
+      </c>
+      <c r="H8" s="19">
         <v>0.26</v>
       </c>
       <c r="I8">
         <v>0.81</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="23">
         <v>5</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>107</v>
-      </c>
-      <c r="M8" s="35">
+        <v>474</v>
+      </c>
+      <c r="M8" s="19">
         <v>0.25</v>
       </c>
       <c r="N8">
         <v>0.82</v>
       </c>
-      <c r="P8" s="39">
+      <c r="P8" s="23">
         <v>5</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>418</v>
-      </c>
-      <c r="R8" s="35">
+        <v>282</v>
+      </c>
+      <c r="R8" s="19">
         <v>0.34</v>
       </c>
       <c r="S8">
@@ -2224,86 +2279,86 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A9" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="45"/>
-      <c r="F9" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="K9" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="P9" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
+      <c r="A9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="F9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="K9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="P9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A10" s="39">
+      <c r="A10" s="23">
         <v>20</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="19">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>11</v>
-      </c>
-      <c r="C10" s="45">
+        <v>638</v>
+      </c>
+      <c r="C10" s="19">
         <v>1.3</v>
       </c>
       <c r="D10">
         <v>0.7</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="27">
         <v>20</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="18">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>631</v>
-      </c>
-      <c r="H10" s="29">
+        <v>952</v>
+      </c>
+      <c r="H10" s="18">
         <v>1.2</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="26">
         <v>0.74</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="27">
         <v>20</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="18">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>526</v>
-      </c>
-      <c r="M10" s="29">
+        <v>230</v>
+      </c>
+      <c r="M10" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="N10" s="42">
+      <c r="N10" s="26">
         <v>0.6</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="27">
         <v>20</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="Q10" s="18">
         <f ca="1">RANDBETWEEN(1,1000)</f>
-        <v>987</v>
-      </c>
-      <c r="R10" s="29">
+        <v>312</v>
+      </c>
+      <c r="R10" s="18">
         <v>3.4</v>
       </c>
-      <c r="S10" s="42">
+      <c r="S10" s="26">
         <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>